<commit_message>
updates into tables, restarting new video, a little bit of formatting
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
+    <workbookView xWindow="30180" yWindow="340" windowWidth="38400" windowHeight="20060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -866,8 +871,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1220,20 +1225,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A152"/>
+    <sheetView tabSelected="1" topLeftCell="B107" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="82.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
-    <col min="7" max="7" width="101.42578125" customWidth="1"/>
+    <col min="7" max="7" width="101.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:7">
@@ -4549,7 +4554,7 @@
         <v>&lt;a id='131' href='#'&gt;131 - Bavagaru Bagunnara? - 1998&lt;/a&gt;&lt;br&gt;</v>
       </c>
       <c r="C134" t="str">
-        <f t="shared" ref="C133:C152" si="8">SUBSTITUTE($G134, "https://www.youtube.com/watch?v=", "")</f>
+        <f t="shared" ref="C134:C152" si="8">SUBSTITUTE($G134, "https://www.youtube.com/watch?v=", "")</f>
         <v>dVwjpyIJAwc</v>
       </c>
       <c r="D134" s="1">
@@ -5177,29 +5182,44 @@
     <hyperlink ref="F152" r:id="rId140" tooltip="Magadheera" display="http://en.wikipedia.org/wiki/Magadheera"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>